<commit_message>
New Scripts are added
</commit_message>
<xml_diff>
--- a/testData/TutorialsNinja Web Application - Test Cases (Complete and Final).xlsx
+++ b/testData/TutorialsNinja Web Application - Test Cases (Complete and Final).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="914" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="914" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Vesion History" sheetId="2" r:id="rId1"/>
@@ -9656,7 +9656,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13991,7 +13991,7 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -15093,8 +15093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -16077,7 +16077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -16480,7 +16480,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -20425,8 +20425,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -22897,9 +22897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -23083,7 +23081,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -23809,7 +23807,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -24211,7 +24209,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>